<commit_message>
Añadidos datos jornada 20 y corregidos errores
</commit_message>
<xml_diff>
--- a/data/classification_J_19.xlsx
+++ b/data/classification_J_19.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="classification_J_19" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="classification_J_19" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -501,7 +501,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -526,12 +526,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>17</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>+25</t>
+          <t>+24</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -556,12 +556,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -586,12 +586,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>+16</t>
+          <t>+17</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>41</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -636,12 +636,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>23</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>+11</t>
+          <t>+9</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -661,12 +661,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Rayo Vallecano</t>
+          <t xml:space="preserve"> Atlético Madrid</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -676,32 +676,32 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>22</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>+8</t>
+          <t>+9</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>32</t>
         </is>
       </c>
     </row>
@@ -716,12 +716,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Atlético Madrid</t>
+          <t xml:space="preserve"> Barcelona</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -731,17 +731,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -751,12 +751,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>+7</t>
+          <t>+8</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>31</t>
         </is>
       </c>
     </row>
@@ -771,47 +771,47 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Real Sociedad</t>
+          <t xml:space="preserve"> Rayo Vallecano</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
           <t>20</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+6</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
     </row>
@@ -826,47 +826,47 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Barcelona</t>
+          <t xml:space="preserve"> Real Sociedad</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>21</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>21</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>+7</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>30</t>
         </is>
       </c>
     </row>
@@ -881,12 +881,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Valencia</t>
+          <t xml:space="preserve"> Villarreal</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -901,22 +901,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>20</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>+4</t>
+          <t>+11</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -936,17 +936,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Villarreal</t>
+          <t xml:space="preserve"> Valencia</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -961,22 +961,22 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>31</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>28</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>+6</t>
+          <t>+3</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>28</t>
         </is>
       </c>
     </row>
@@ -996,42 +996,42 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>20</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
       <c r="H11" t="inlineStr">
         <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
           <t>17</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
-      </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>+1</t>
+          <t>+3</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>27</t>
         </is>
       </c>
     </row>
@@ -1051,12 +1051,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1071,22 +1071,22 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>22</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>22</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>-1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>26</t>
         </is>
       </c>
     </row>
@@ -1101,47 +1101,47 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Granada</t>
+          <t xml:space="preserve"> Celta Vigo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
           <t>23</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>-3</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>22</t>
         </is>
       </c>
     </row>
@@ -1156,12 +1156,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Osasuna</t>
+          <t xml:space="preserve"> Granada</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1171,7 +1171,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1181,22 +1181,22 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>26</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>-5</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>23</t>
         </is>
       </c>
     </row>
@@ -1211,47 +1211,47 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celta Vigo</t>
+          <t xml:space="preserve"> Osasuna</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
           <t>18</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
       <c r="I15" t="inlineStr">
         <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
           <t>22</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>20</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1296,12 +1296,12 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>28</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>-10</t>
+          <t>-11</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1326,42 +1326,42 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>-7</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
           <t>18</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>-8</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>15</t>
         </is>
       </c>
     </row>
@@ -1381,29 +1381,29 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
           <t>18</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
       <c r="I18" t="inlineStr">
         <is>
           <t>27</t>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1456,12 +1456,12 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>30</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>16</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1516,12 +1516,12 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>32</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>-16</t>
+          <t>-17</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1571,12 +1571,12 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>41</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>-17</t>
+          <t>-22</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">

</xml_diff>